<commit_message>
calorimetry : scripts : postproc WIP
</commit_message>
<xml_diff>
--- a/input/calorimetry/ds.4.overfilled/data.xlsx
+++ b/input/calorimetry/ds.4.overfilled/data.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="4"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="input_stoich_coefficients" sheetId="1" state="visible" r:id="rId2"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="25">
   <si>
     <t xml:space="preserve">H</t>
   </si>
@@ -106,10 +106,11 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="3">
+  <numFmts count="4">
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="0.000000E+00"/>
     <numFmt numFmtId="166" formatCode="0.000E+00"/>
+    <numFmt numFmtId="167" formatCode="0.00E+00"/>
   </numFmts>
   <fonts count="4">
     <font>
@@ -177,7 +178,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -187,6 +188,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -210,7 +215,7 @@
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="1" sqref="AS2 A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -307,7 +312,7 @@
   <dimension ref="A1:A5"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="1" sqref="AS2 A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -356,10 +361,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G63"/>
+  <dimension ref="A1:G1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A27" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A26" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A47" activeCellId="1" sqref="AS2 A47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1069,247 +1074,233 @@
       </c>
       <c r="G46" s="1"/>
     </row>
-    <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="0" t="n">
-        <v>0.001047</v>
+        <v>0.00120095141700405</v>
       </c>
       <c r="B47" s="0" t="n">
-        <v>0.001047</v>
-      </c>
-      <c r="C47" s="0" t="n">
-        <v>1E-016</v>
+        <v>0.00103853513825829</v>
+      </c>
+      <c r="C47" s="3" t="n">
+        <v>1E-019</v>
       </c>
       <c r="D47" s="2" t="s">
         <v>12</v>
       </c>
       <c r="G47" s="1"/>
     </row>
-    <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="0" t="n">
-        <v>0.00120095141700405</v>
+        <v>0.00148727300480257</v>
       </c>
       <c r="B48" s="0" t="n">
-        <v>0.00103853513825829</v>
-      </c>
-      <c r="C48" s="0" t="n">
-        <v>1E-016</v>
+        <v>0.00102276790437785</v>
+      </c>
+      <c r="C48" s="3" t="n">
+        <v>1E-019</v>
       </c>
       <c r="D48" s="2" t="s">
         <v>12</v>
       </c>
       <c r="G48" s="1"/>
     </row>
-    <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="0" t="n">
-        <v>0.00148727300480257</v>
+        <v>0.00176924760493209</v>
       </c>
       <c r="B49" s="0" t="n">
-        <v>0.00102276790437785</v>
-      </c>
-      <c r="C49" s="0" t="n">
-        <v>1E-016</v>
+        <v>0.00100724005157859</v>
+      </c>
+      <c r="C49" s="3" t="n">
+        <v>1E-019</v>
       </c>
       <c r="D49" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="G49" s="1"/>
-    </row>
-    <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="0" t="n">
-        <v>0.00176924760493209</v>
+        <v>0.00204694121416895</v>
       </c>
       <c r="B50" s="0" t="n">
-        <v>0.00100724005157859</v>
-      </c>
-      <c r="C50" s="0" t="n">
-        <v>1E-016</v>
+        <v>0.000991947945532358</v>
+      </c>
+      <c r="C50" s="3" t="n">
+        <v>1E-019</v>
       </c>
       <c r="D50" s="2" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="0" t="n">
-        <v>0.00204694121416895</v>
+        <v>0.00232041882731415</v>
       </c>
       <c r="B51" s="0" t="n">
-        <v>0.000991947945532358</v>
-      </c>
-      <c r="C51" s="0" t="n">
-        <v>1E-016</v>
+        <v>0.00097688800708804</v>
+      </c>
+      <c r="C51" s="3" t="n">
+        <v>1E-019</v>
       </c>
       <c r="D51" s="2" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="52" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="0" t="n">
-        <v>0.00232041882731415</v>
+        <v>0.00258974445240554</v>
       </c>
       <c r="B52" s="0" t="n">
-        <v>0.00097688800708804</v>
-      </c>
-      <c r="C52" s="0" t="n">
-        <v>1E-016</v>
+        <v>0.00096205671143387</v>
+      </c>
+      <c r="C52" s="3" t="n">
+        <v>1E-019</v>
       </c>
       <c r="D52" s="2" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="53" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="0" t="n">
-        <v>0.00258974445240554</v>
+        <v>0.00285498112569898</v>
       </c>
       <c r="B53" s="0" t="n">
-        <v>0.00096205671143387</v>
-      </c>
-      <c r="C53" s="0" t="n">
-        <v>1E-016</v>
+        <v>0.000947450587272424</v>
+      </c>
+      <c r="C53" s="3" t="n">
+        <v>1E-019</v>
       </c>
       <c r="D53" s="2" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="54" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="0" t="n">
-        <v>0.00285498112569898</v>
+        <v>0.00311619092642217</v>
       </c>
       <c r="B54" s="0" t="n">
-        <v>0.000947450587272424</v>
-      </c>
-      <c r="C54" s="0" t="n">
-        <v>1E-016</v>
+        <v>0.000933066216008167</v>
+      </c>
+      <c r="C54" s="3" t="n">
+        <v>1E-019</v>
       </c>
       <c r="D54" s="2" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="55" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="0" t="n">
-        <v>0.00311619092642217</v>
+        <v>0.00337343499130443</v>
       </c>
       <c r="B55" s="0" t="n">
-        <v>0.000933066216008167</v>
-      </c>
-      <c r="C55" s="0" t="n">
-        <v>1E-016</v>
+        <v>0.000918900230947314</v>
+      </c>
+      <c r="C55" s="3" t="n">
+        <v>1E-019</v>
       </c>
       <c r="D55" s="2" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="56" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="0" t="n">
-        <v>0.00337343499130443</v>
+        <v>0.00362677352888584</v>
       </c>
       <c r="B56" s="0" t="n">
-        <v>0.000918900230947314</v>
-      </c>
-      <c r="C56" s="0" t="n">
-        <v>1E-016</v>
+        <v>0.000904949316509855</v>
+      </c>
+      <c r="C56" s="3" t="n">
+        <v>1E-019</v>
       </c>
       <c r="D56" s="2" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="57" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="0" t="n">
-        <v>0.00362677352888584</v>
+        <v>0.00387626583360923</v>
       </c>
       <c r="B57" s="0" t="n">
-        <v>0.000904949316509855</v>
-      </c>
-      <c r="C57" s="0" t="n">
-        <v>1E-016</v>
+        <v>0.000891210207453531</v>
+      </c>
+      <c r="C57" s="3" t="n">
+        <v>1E-019</v>
       </c>
       <c r="D57" s="2" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="58" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="0" t="n">
-        <v>0.00387626583360923</v>
+        <v>0.00412197029969816</v>
       </c>
       <c r="B58" s="0" t="n">
-        <v>0.000891210207453531</v>
-      </c>
-      <c r="C58" s="0" t="n">
-        <v>1E-016</v>
+        <v>0.000877679688109601</v>
+      </c>
+      <c r="C58" s="3" t="n">
+        <v>1E-019</v>
       </c>
       <c r="D58" s="2" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="59" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="59" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="0" t="n">
-        <v>0.00412197029969816</v>
+        <v>0.0043639444348242</v>
       </c>
       <c r="B59" s="0" t="n">
-        <v>0.000877679688109601</v>
-      </c>
-      <c r="C59" s="0" t="n">
-        <v>1E-016</v>
+        <v>0.000864354591630204</v>
+      </c>
+      <c r="C59" s="3" t="n">
+        <v>1E-019</v>
       </c>
       <c r="D59" s="2" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="60" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="60" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="0" t="n">
-        <v>0.0043639444348242</v>
+        <v>0.00460224487356675</v>
       </c>
       <c r="B60" s="0" t="n">
-        <v>0.000864354591630204</v>
-      </c>
-      <c r="C60" s="0" t="n">
-        <v>1E-016</v>
+        <v>0.000851231799247154</v>
+      </c>
+      <c r="C60" s="3" t="n">
+        <v>1E-019</v>
       </c>
       <c r="D60" s="2" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="61" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="0" t="n">
-        <v>0.00460224487356675</v>
+        <v>0.00483692739066846</v>
       </c>
       <c r="B61" s="0" t="n">
-        <v>0.000851231799247154</v>
-      </c>
-      <c r="C61" s="0" t="n">
-        <v>1E-016</v>
+        <v>0.000838308239541985</v>
+      </c>
+      <c r="C61" s="3" t="n">
+        <v>1E-019</v>
       </c>
       <c r="D61" s="2" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="62" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="62" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="0" t="n">
-        <v>0.00483692739066846</v>
+        <v>0.00506804691408949</v>
       </c>
       <c r="B62" s="0" t="n">
-        <v>0.000838308239541985</v>
-      </c>
-      <c r="C62" s="0" t="n">
-        <v>1E-016</v>
+        <v>0.000825580887727076</v>
+      </c>
+      <c r="C62" s="3" t="n">
+        <v>1E-019</v>
       </c>
       <c r="D62" s="2" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="63" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A63" s="0" t="n">
-        <v>0.00506804691408949</v>
-      </c>
-      <c r="B63" s="0" t="n">
-        <v>0.000825580887727076</v>
-      </c>
-      <c r="C63" s="0" t="n">
-        <v>1E-016</v>
-      </c>
-      <c r="D63" s="2" t="s">
-        <v>12</v>
-      </c>
-    </row>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
@@ -1326,20 +1317,21 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:BH5"/>
+  <dimension ref="A1:BG5"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="AE1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="BA13" activeCellId="0" sqref="BA13"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="AM1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="AS2" activeCellId="0" sqref="AS2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="60" min="1" style="0" width="8.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="61" min="61" style="0" width="8.53"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="62" style="0" width="8.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="59" min="1" style="0" width="8.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="60" min="60" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1023" min="61" style="0" width="8.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1024" style="0" width="9.14"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
         <v>13</v>
       </c>
@@ -1517,11 +1509,8 @@
       <c r="BG1" s="0" t="n">
         <v>58</v>
       </c>
-      <c r="BH1" s="0" t="n">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
         <v>14</v>
       </c>
@@ -1655,55 +1644,52 @@
         <v>0.004</v>
       </c>
       <c r="AS2" s="0" t="n">
-        <v>0.002</v>
+        <v>0.015</v>
       </c>
       <c r="AT2" s="0" t="n">
-        <v>0.00600000000000001</v>
+        <v>0.015</v>
       </c>
       <c r="AU2" s="0" t="n">
-        <v>0.0149999999999999</v>
+        <v>0.015</v>
       </c>
       <c r="AV2" s="0" t="n">
-        <v>0.0150000000000001</v>
+        <v>0.015</v>
       </c>
       <c r="AW2" s="0" t="n">
-        <v>0.0149999999999999</v>
+        <v>0.015</v>
       </c>
       <c r="AX2" s="0" t="n">
-        <v>0.0150000000000001</v>
+        <v>0.015</v>
       </c>
       <c r="AY2" s="0" t="n">
-        <v>0.0149999999999999</v>
+        <v>0.015</v>
       </c>
       <c r="AZ2" s="0" t="n">
-        <v>0.0150000000000001</v>
+        <v>0.015</v>
       </c>
       <c r="BA2" s="0" t="n">
-        <v>0.0149999999999999</v>
+        <v>0.015</v>
       </c>
       <c r="BB2" s="0" t="n">
-        <v>0.0150000000000001</v>
+        <v>0.015</v>
       </c>
       <c r="BC2" s="0" t="n">
-        <v>0.0149999999999999</v>
+        <v>0.015</v>
       </c>
       <c r="BD2" s="0" t="n">
-        <v>0.0149999999999999</v>
+        <v>0.015</v>
       </c>
       <c r="BE2" s="0" t="n">
-        <v>0.0150000000000001</v>
+        <v>0.015</v>
       </c>
       <c r="BF2" s="0" t="n">
-        <v>0.0149999999999999</v>
+        <v>0.015</v>
       </c>
       <c r="BG2" s="0" t="n">
-        <v>0.0150000000000001</v>
-      </c>
-      <c r="BH2" s="0" t="n">
-        <v>0.0149999999999999</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>0.015</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
         <v>15</v>
       </c>
@@ -1837,55 +1823,52 @@
         <v>3.4E-005</v>
       </c>
       <c r="AS3" s="0" t="n">
-        <v>0.000625</v>
+        <v>0.000688</v>
       </c>
       <c r="AT3" s="0" t="n">
-        <v>0.000688</v>
+        <v>0.000251</v>
       </c>
       <c r="AU3" s="0" t="n">
-        <v>0.000251</v>
+        <v>0.000149</v>
       </c>
       <c r="AV3" s="0" t="n">
-        <v>0.000149</v>
+        <v>0.000107</v>
       </c>
       <c r="AW3" s="0" t="n">
-        <v>0.000107</v>
+        <v>8.5E-005</v>
       </c>
       <c r="AX3" s="0" t="n">
-        <v>8.5E-005</v>
+        <v>7.8E-005</v>
       </c>
       <c r="AY3" s="0" t="n">
-        <v>7.8E-005</v>
+        <v>6.7E-005</v>
       </c>
       <c r="AZ3" s="0" t="n">
-        <v>6.7E-005</v>
+        <v>5.8E-005</v>
       </c>
       <c r="BA3" s="0" t="n">
-        <v>5.8E-005</v>
+        <v>5.4E-005</v>
       </c>
       <c r="BB3" s="0" t="n">
-        <v>5.4E-005</v>
+        <v>5.3E-005</v>
       </c>
       <c r="BC3" s="0" t="n">
         <v>5.3E-005</v>
       </c>
       <c r="BD3" s="0" t="n">
-        <v>5.3E-005</v>
+        <v>4.8E-005</v>
       </c>
       <c r="BE3" s="0" t="n">
-        <v>4.8E-005</v>
+        <v>4.1E-005</v>
       </c>
       <c r="BF3" s="0" t="n">
-        <v>4.1E-005</v>
+        <v>3.8E-005</v>
       </c>
       <c r="BG3" s="0" t="n">
         <v>3.8E-005</v>
       </c>
-      <c r="BH3" s="0" t="n">
-        <v>3.8E-005</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
         <v>16</v>
       </c>
@@ -2063,11 +2046,8 @@
       <c r="BG4" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="BH4" s="0" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
         <v>17</v>
       </c>
@@ -2243,9 +2223,6 @@
         <v>1E-009</v>
       </c>
       <c r="BG5" s="0" t="n">
-        <v>1E-009</v>
-      </c>
-      <c r="BH5" s="0" t="n">
         <v>1E-009</v>
       </c>
     </row>
@@ -2267,8 +2244,8 @@
   </sheetPr>
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A4" activeCellId="1" sqref="AS2 A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2319,7 +2296,7 @@
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
+      <selection pane="topLeft" activeCell="A4" activeCellId="1" sqref="AS2 A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>